<commit_message>
ITC-?? - Add Real Estate Administration Massive Export class and XSD schema for Real Estate Development.
</commit_message>
<xml_diff>
--- a/public/templates/plantillaAdministracionCuentasBancarias.xlsx
+++ b/public/templates/plantillaAdministracionCuentasBancarias.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-24.04\home\jrrmelecio\projects\ITConsultores\pld\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jrrme\Downloads\Actualizar Plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01E7E7E1-5794-4E52-AF60-4AA6AF4FB948}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A4C9CFE-EEEF-482F-B446-97F092828C7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="3" r:id="rId1"/>
@@ -190,7 +190,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="986" uniqueCount="953">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="988" uniqueCount="955">
   <si>
     <t>RFC</t>
   </si>
@@ -3049,6 +3049,12 @@
   </si>
   <si>
     <t>Numero de operaciones</t>
+  </si>
+  <si>
+    <t>route_param</t>
+  </si>
+  <si>
+    <t>bank_account_management</t>
   </si>
 </sst>
 </file>
@@ -3322,10 +3328,14 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3334,26 +3344,22 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3772,194 +3778,194 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="10"/>
-      <c r="C1" s="10"/>
-      <c r="D1" s="9" t="s">
+      <c r="B1" s="19"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="10"/>
-      <c r="F1" s="9" t="s">
+      <c r="E1" s="19"/>
+      <c r="F1" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="11" t="s">
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+      <c r="Y1" s="19"/>
+      <c r="Z1" s="19"/>
+      <c r="AA1" s="19"/>
+      <c r="AB1" s="13" t="s">
         <v>615</v>
       </c>
-      <c r="AC1" s="12"/>
-      <c r="AD1" s="12"/>
-      <c r="AE1" s="12"/>
-      <c r="AF1" s="12"/>
-      <c r="AG1" s="12"/>
-      <c r="AH1" s="12"/>
-      <c r="AI1" s="12"/>
-      <c r="AJ1" s="12"/>
-      <c r="AK1" s="12"/>
-      <c r="AL1" s="12"/>
-      <c r="AM1" s="12"/>
-      <c r="AN1" s="12"/>
-      <c r="AO1" s="12"/>
-      <c r="AP1" s="12"/>
-      <c r="AQ1" s="12"/>
-      <c r="AR1" s="11" t="s">
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="14"/>
+      <c r="AI1" s="14"/>
+      <c r="AJ1" s="14"/>
+      <c r="AK1" s="14"/>
+      <c r="AL1" s="14"/>
+      <c r="AM1" s="14"/>
+      <c r="AN1" s="14"/>
+      <c r="AO1" s="14"/>
+      <c r="AP1" s="14"/>
+      <c r="AQ1" s="14"/>
+      <c r="AR1" s="13" t="s">
         <v>630</v>
       </c>
-      <c r="AS1" s="12"/>
-      <c r="AT1" s="12"/>
-      <c r="AU1" s="12"/>
-      <c r="AV1" s="12"/>
-      <c r="AW1" s="12"/>
-      <c r="AX1" s="12"/>
-      <c r="AY1" s="12"/>
-      <c r="AZ1" s="12"/>
-      <c r="BA1" s="12"/>
-      <c r="BB1" s="12"/>
-      <c r="BC1" s="12"/>
-      <c r="BD1" s="12"/>
-      <c r="BE1" s="12"/>
-      <c r="BF1" s="11" t="s">
+      <c r="AS1" s="14"/>
+      <c r="AT1" s="14"/>
+      <c r="AU1" s="14"/>
+      <c r="AV1" s="14"/>
+      <c r="AW1" s="14"/>
+      <c r="AX1" s="14"/>
+      <c r="AY1" s="14"/>
+      <c r="AZ1" s="14"/>
+      <c r="BA1" s="14"/>
+      <c r="BB1" s="14"/>
+      <c r="BC1" s="14"/>
+      <c r="BD1" s="14"/>
+      <c r="BE1" s="14"/>
+      <c r="BF1" s="13" t="s">
         <v>637</v>
       </c>
-      <c r="BG1" s="12"/>
-      <c r="BH1" s="12"/>
-      <c r="BI1" s="12"/>
-      <c r="BJ1" s="12"/>
-      <c r="BK1" s="9" t="s">
+      <c r="BG1" s="14"/>
+      <c r="BH1" s="14"/>
+      <c r="BI1" s="14"/>
+      <c r="BJ1" s="14"/>
+      <c r="BK1" s="18" t="s">
         <v>683</v>
       </c>
-      <c r="BL1" s="10"/>
-      <c r="BM1" s="10"/>
-      <c r="BN1" s="10"/>
-      <c r="BO1" s="10"/>
-      <c r="BP1" s="10"/>
-      <c r="BQ1" s="10"/>
+      <c r="BL1" s="19"/>
+      <c r="BM1" s="19"/>
+      <c r="BN1" s="19"/>
+      <c r="BO1" s="19"/>
+      <c r="BP1" s="19"/>
+      <c r="BQ1" s="19"/>
     </row>
     <row r="2" spans="1:69" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="9" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="9" t="s">
+      <c r="E2" s="19"/>
+      <c r="F2" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="9" t="s">
+      <c r="G2" s="19"/>
+      <c r="H2" s="19"/>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="K2" s="19"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="18" t="s">
         <v>470</v>
       </c>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="14" t="s">
+      <c r="O2" s="19"/>
+      <c r="P2" s="19"/>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="10" t="s">
         <v>610</v>
       </c>
-      <c r="T2" s="15"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="14" t="s">
+      <c r="T2" s="11"/>
+      <c r="U2" s="15"/>
+      <c r="V2" s="10" t="s">
         <v>613</v>
       </c>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15"/>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="14" t="s">
+      <c r="W2" s="11"/>
+      <c r="X2" s="11"/>
+      <c r="Y2" s="11"/>
+      <c r="Z2" s="11"/>
+      <c r="AA2" s="11"/>
+      <c r="AB2" s="10" t="s">
         <v>616</v>
       </c>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="15"/>
-      <c r="AF2" s="15"/>
-      <c r="AG2" s="14" t="s">
+      <c r="AC2" s="11"/>
+      <c r="AD2" s="11"/>
+      <c r="AE2" s="11"/>
+      <c r="AF2" s="11"/>
+      <c r="AG2" s="10" t="s">
         <v>622</v>
       </c>
-      <c r="AH2" s="15"/>
-      <c r="AI2" s="15"/>
-      <c r="AJ2" s="15"/>
-      <c r="AK2" s="15"/>
-      <c r="AL2" s="15"/>
-      <c r="AM2" s="15"/>
-      <c r="AN2" s="15"/>
-      <c r="AO2" s="14" t="s">
+      <c r="AH2" s="11"/>
+      <c r="AI2" s="11"/>
+      <c r="AJ2" s="11"/>
+      <c r="AK2" s="11"/>
+      <c r="AL2" s="11"/>
+      <c r="AM2" s="11"/>
+      <c r="AN2" s="11"/>
+      <c r="AO2" s="10" t="s">
         <v>626</v>
       </c>
-      <c r="AP2" s="15"/>
-      <c r="AQ2" s="15"/>
-      <c r="AR2" s="14" t="s">
+      <c r="AP2" s="11"/>
+      <c r="AQ2" s="11"/>
+      <c r="AR2" s="10" t="s">
         <v>631</v>
       </c>
-      <c r="AS2" s="15"/>
-      <c r="AT2" s="15"/>
-      <c r="AU2" s="15"/>
-      <c r="AV2" s="15"/>
-      <c r="AW2" s="15"/>
-      <c r="AX2" s="15"/>
-      <c r="AY2" s="14" t="s">
+      <c r="AS2" s="11"/>
+      <c r="AT2" s="11"/>
+      <c r="AU2" s="11"/>
+      <c r="AV2" s="11"/>
+      <c r="AW2" s="11"/>
+      <c r="AX2" s="11"/>
+      <c r="AY2" s="10" t="s">
         <v>470</v>
       </c>
-      <c r="AZ2" s="15"/>
-      <c r="BA2" s="15"/>
-      <c r="BB2" s="15"/>
-      <c r="BC2" s="14" t="s">
+      <c r="AZ2" s="11"/>
+      <c r="BA2" s="11"/>
+      <c r="BB2" s="11"/>
+      <c r="BC2" s="10" t="s">
         <v>610</v>
       </c>
-      <c r="BD2" s="15"/>
-      <c r="BE2" s="15"/>
-      <c r="BF2" s="17" t="s">
+      <c r="BD2" s="11"/>
+      <c r="BE2" s="11"/>
+      <c r="BF2" s="9" t="s">
         <v>951</v>
       </c>
-      <c r="BG2" s="14" t="s">
+      <c r="BG2" s="10" t="s">
         <v>632</v>
       </c>
-      <c r="BH2" s="15"/>
-      <c r="BI2" s="15"/>
-      <c r="BJ2" s="16"/>
-      <c r="BK2" s="18" t="s">
+      <c r="BH2" s="11"/>
+      <c r="BI2" s="11"/>
+      <c r="BJ2" s="15"/>
+      <c r="BK2" s="16" t="s">
         <v>693</v>
       </c>
-      <c r="BL2" s="19"/>
-      <c r="BM2" s="18" t="s">
+      <c r="BL2" s="17"/>
+      <c r="BM2" s="16" t="s">
         <v>689</v>
       </c>
-      <c r="BN2" s="20"/>
-      <c r="BO2" s="19"/>
-      <c r="BP2" s="20" t="s">
+      <c r="BN2" s="12"/>
+      <c r="BO2" s="17"/>
+      <c r="BP2" s="12" t="s">
         <v>690</v>
       </c>
-      <c r="BQ2" s="20"/>
+      <c r="BQ2" s="12"/>
     </row>
     <row r="3" spans="1:69" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -11266,16 +11272,6 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="AR2:AX2"/>
-    <mergeCell ref="BP2:BQ2"/>
-    <mergeCell ref="BC2:BE2"/>
-    <mergeCell ref="AR1:BE1"/>
-    <mergeCell ref="BG2:BJ2"/>
-    <mergeCell ref="BF1:BJ1"/>
-    <mergeCell ref="BK2:BL2"/>
-    <mergeCell ref="BM2:BO2"/>
-    <mergeCell ref="BK1:BQ1"/>
-    <mergeCell ref="AY2:BB2"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A1:C1"/>
     <mergeCell ref="AO2:AQ2"/>
@@ -11289,6 +11285,16 @@
     <mergeCell ref="AB2:AF2"/>
     <mergeCell ref="AG2:AN2"/>
     <mergeCell ref="AB1:AQ1"/>
+    <mergeCell ref="AR2:AX2"/>
+    <mergeCell ref="BP2:BQ2"/>
+    <mergeCell ref="BC2:BE2"/>
+    <mergeCell ref="AR1:BE1"/>
+    <mergeCell ref="BG2:BJ2"/>
+    <mergeCell ref="BF1:BJ1"/>
+    <mergeCell ref="BK2:BL2"/>
+    <mergeCell ref="BM2:BO2"/>
+    <mergeCell ref="BK1:BQ1"/>
+    <mergeCell ref="AY2:BB2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -11297,61 +11303,61 @@
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="10">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{CE855D05-F0A5-423B-9E26-432A86BC6A16}">
           <x14:formula1>
-            <xm:f>Configuracion!$C$2:$C$28</xm:f>
+            <xm:f>Configuracion!$D$2:$D$28</xm:f>
           </x14:formula1>
           <xm:sqref>D4:D103</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4BAB6183-5B6C-4969-BCD1-31BC352978E5}">
           <x14:formula1>
-            <xm:f>Configuracion!$E$2:$E$250</xm:f>
+            <xm:f>Configuracion!$F$2:$F$250</xm:f>
           </x14:formula1>
-          <xm:sqref>L4:L103 Q4:Q103 AG4:AG103 AO4:AO103 AX4 AX6:AX103 BB4:BB103</xm:sqref>
+          <xm:sqref>L4:L103 BB4:BB103 AX6:AX103 AX4 AO4:AO103 AG4:AG103 Q4:Q103</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{F71B2D5A-2E28-4A46-8FC7-681F75C3EE49}">
           <x14:formula1>
-            <xm:f>Configuracion!$G$2:$G$168</xm:f>
+            <xm:f>Configuracion!$H$2:$H$168</xm:f>
           </x14:formula1>
           <xm:sqref>M4:M103</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8CC1387C-5191-4E4F-AE71-68FA034F7A48}">
           <x14:formula1>
-            <xm:f>Configuracion!$I$2:$I$137</xm:f>
+            <xm:f>Configuracion!$J$2:$J$137</xm:f>
           </x14:formula1>
           <xm:sqref>R4:R103</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{9CD4616A-618A-45A9-B00C-74CD8A4AEFC5}">
           <x14:formula1>
-            <xm:f>Configuracion!$K$2:$K$4</xm:f>
+            <xm:f>Configuracion!$L$2:$L$4</xm:f>
           </x14:formula1>
           <xm:sqref>BG4:BG103</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{41CD14C3-02EF-4CB5-88D7-1075F8944DD3}">
           <x14:formula1>
-            <xm:f>Configuracion!$M$2:$M$41</xm:f>
+            <xm:f>Configuracion!$N$2:$N$41</xm:f>
           </x14:formula1>
           <xm:sqref>BH4:BH103</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{05E0D2E7-3946-4076-A8F3-BCCE9145F876}">
           <x14:formula1>
-            <xm:f>Configuracion!$O$2:$O$18</xm:f>
+            <xm:f>Configuracion!$P$2:$P$18</xm:f>
           </x14:formula1>
           <xm:sqref>BL4:BL103</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{C2009687-FFE8-49E0-B28F-0E1FB1C6E908}">
           <x14:formula1>
-            <xm:f>Configuracion!$Q$2:$Q$52</xm:f>
+            <xm:f>Configuracion!$R$2:$R$52</xm:f>
           </x14:formula1>
           <xm:sqref>BM4:BM103</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4BCBBD3C-994F-4F93-BC4B-8E34AE637EE7}">
           <x14:formula1>
-            <xm:f>Configuracion!$S$2:$S$185</xm:f>
+            <xm:f>Configuracion!$T$2:$T$185</xm:f>
           </x14:formula1>
           <xm:sqref>BP4:BP103</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8F2EEA0A-D29B-4ACC-99E7-F14B803E4A52}">
           <x14:formula1>
-            <xm:f>Configuracion!$U$2:$U$3</xm:f>
+            <xm:f>Configuracion!$V$2:$V$3</xm:f>
           </x14:formula1>
           <xm:sqref>C4:C103</xm:sqref>
         </x14:dataValidation>
@@ -11363,3195 +11369,3202 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:U250"/>
+  <dimension ref="A1:V250"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="T9" sqref="T9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.42578125" style="3"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>301</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>469</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>641</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>682</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>685</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>762</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>947</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>948</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>954</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>52</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>302</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>302</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>638</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>642</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>694</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>711</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>763</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>949</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>53</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>303</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>474</v>
       </c>
-      <c r="K3" s="5" t="s">
+      <c r="L3" s="5" t="s">
         <v>639</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>643</v>
       </c>
-      <c r="O3" t="s">
+      <c r="P3" t="s">
         <v>695</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>712</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>764</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>950</v>
       </c>
     </row>
-    <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="D4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>54</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>304</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>475</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>640</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>644</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
         <v>696</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>713</v>
       </c>
-      <c r="S4" t="s">
+      <c r="T4" t="s">
         <v>765</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="5" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="D5" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>55</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>305</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>476</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>645</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
         <v>697</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>714</v>
       </c>
-      <c r="S5" t="s">
+      <c r="T5" t="s">
         <v>766</v>
       </c>
     </row>
-    <row r="6" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+    <row r="6" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>56</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>306</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>477</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>646</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
         <v>698</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>715</v>
       </c>
-      <c r="S6" t="s">
+      <c r="T6" t="s">
         <v>767</v>
       </c>
     </row>
-    <row r="7" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+    <row r="7" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4" t="s">
+      <c r="D7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>57</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>307</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>478</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>647</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
         <v>699</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>716</v>
       </c>
-      <c r="S7" t="s">
+      <c r="T7" t="s">
         <v>768</v>
       </c>
     </row>
-    <row r="8" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C8" s="4" t="s">
+    <row r="8" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>58</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>308</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>479</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>648</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
         <v>700</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>717</v>
       </c>
-      <c r="S8" t="s">
+      <c r="T8" t="s">
         <v>769</v>
       </c>
     </row>
-    <row r="9" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C9" s="4" t="s">
+    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>59</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>309</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>480</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>649</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
         <v>701</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>718</v>
       </c>
-      <c r="S9" t="s">
+      <c r="T9" t="s">
         <v>770</v>
       </c>
-      <c r="T9" s="6"/>
-    </row>
-    <row r="10" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="4" t="s">
+      <c r="U9" s="6"/>
+    </row>
+    <row r="10" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>60</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>310</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>481</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>650</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
         <v>702</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>719</v>
       </c>
-      <c r="S10" t="s">
+      <c r="T10" t="s">
         <v>771</v>
       </c>
     </row>
-    <row r="11" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="4" t="s">
+    <row r="11" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>61</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>311</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>482</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>651</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
         <v>703</v>
       </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>720</v>
       </c>
-      <c r="S11" t="s">
+      <c r="T11" t="s">
         <v>772</v>
       </c>
     </row>
-    <row r="12" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="4" t="s">
+    <row r="12" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>62</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>312</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>483</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>652</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
         <v>704</v>
       </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>721</v>
       </c>
-      <c r="S12" t="s">
+      <c r="T12" t="s">
         <v>773</v>
       </c>
     </row>
-    <row r="13" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="4" t="s">
+    <row r="13" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>63</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>313</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>484</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>653</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
         <v>705</v>
       </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>722</v>
       </c>
-      <c r="S13" t="s">
+      <c r="T13" t="s">
         <v>774</v>
       </c>
     </row>
-    <row r="14" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C14" s="4" t="s">
+    <row r="14" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>64</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>314</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>485</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>654</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
         <v>706</v>
       </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>723</v>
       </c>
-      <c r="S14" t="s">
+      <c r="T14" t="s">
         <v>775</v>
       </c>
     </row>
-    <row r="15" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C15" s="4" t="s">
+    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>65</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>315</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>486</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>655</v>
       </c>
-      <c r="O15" t="s">
+      <c r="P15" t="s">
         <v>707</v>
       </c>
-      <c r="Q15" t="s">
+      <c r="R15" t="s">
         <v>724</v>
       </c>
-      <c r="S15" t="s">
+      <c r="T15" t="s">
         <v>776</v>
       </c>
     </row>
-    <row r="16" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C16" s="4" t="s">
+    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>66</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>316</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>487</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>656</v>
       </c>
-      <c r="O16" t="s">
+      <c r="P16" t="s">
         <v>708</v>
       </c>
-      <c r="Q16" t="s">
+      <c r="R16" t="s">
         <v>725</v>
       </c>
-      <c r="S16" t="s">
+      <c r="T16" t="s">
         <v>777</v>
       </c>
     </row>
-    <row r="17" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="4" t="s">
+    <row r="17" spans="4:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>67</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>317</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>488</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>657</v>
       </c>
-      <c r="O17" t="s">
+      <c r="P17" t="s">
         <v>709</v>
       </c>
-      <c r="Q17" t="s">
+      <c r="R17" t="s">
         <v>726</v>
       </c>
-      <c r="S17" t="s">
+      <c r="T17" t="s">
         <v>778</v>
       </c>
     </row>
-    <row r="18" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="4" t="s">
+    <row r="18" spans="4:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>68</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>318</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>489</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>658</v>
       </c>
-      <c r="O18" t="s">
+      <c r="P18" t="s">
         <v>710</v>
       </c>
-      <c r="Q18" t="s">
+      <c r="R18" t="s">
         <v>727</v>
       </c>
-      <c r="S18" t="s">
+      <c r="T18" t="s">
         <v>779</v>
       </c>
     </row>
-    <row r="19" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="4" t="s">
+    <row r="19" spans="4:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>69</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>319</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>490</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>659</v>
       </c>
-      <c r="Q19" t="s">
+      <c r="R19" t="s">
         <v>728</v>
       </c>
-      <c r="S19" t="s">
+      <c r="T19" t="s">
         <v>780</v>
       </c>
     </row>
-    <row r="20" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="4" t="s">
+    <row r="20" spans="4:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>70</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>320</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>491</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>660</v>
       </c>
-      <c r="Q20" t="s">
+      <c r="R20" t="s">
         <v>729</v>
       </c>
-      <c r="S20" t="s">
+      <c r="T20" t="s">
         <v>781</v>
       </c>
     </row>
-    <row r="21" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="4" t="s">
+    <row r="21" spans="4:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>71</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>321</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>492</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>661</v>
       </c>
-      <c r="Q21" t="s">
+      <c r="R21" t="s">
         <v>730</v>
       </c>
-      <c r="S21" t="s">
+      <c r="T21" t="s">
         <v>782</v>
       </c>
     </row>
-    <row r="22" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="4" t="s">
+    <row r="22" spans="4:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="E22" t="s">
+      <c r="F22" t="s">
         <v>72</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>322</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>493</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>662</v>
       </c>
-      <c r="Q22" t="s">
+      <c r="R22" t="s">
         <v>731</v>
       </c>
-      <c r="S22" t="s">
+      <c r="T22" t="s">
         <v>783</v>
       </c>
     </row>
-    <row r="23" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="4" t="s">
+    <row r="23" spans="4:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E23" t="s">
+      <c r="F23" t="s">
         <v>73</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>323</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>494</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>663</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="R23" t="s">
         <v>732</v>
       </c>
-      <c r="S23" t="s">
+      <c r="T23" t="s">
         <v>784</v>
       </c>
     </row>
-    <row r="24" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="4" t="s">
+    <row r="24" spans="4:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E24" t="s">
+      <c r="F24" t="s">
         <v>74</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>324</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>495</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>664</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="R24" t="s">
         <v>733</v>
       </c>
-      <c r="S24" t="s">
+      <c r="T24" t="s">
         <v>785</v>
       </c>
     </row>
-    <row r="25" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="4" t="s">
+    <row r="25" spans="4:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
         <v>75</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>325</v>
       </c>
-      <c r="I25" t="s">
+      <c r="J25" t="s">
         <v>496</v>
       </c>
-      <c r="M25" t="s">
+      <c r="N25" t="s">
         <v>665</v>
       </c>
-      <c r="Q25" t="s">
+      <c r="R25" t="s">
         <v>734</v>
       </c>
-      <c r="S25" t="s">
+      <c r="T25" t="s">
         <v>786</v>
       </c>
     </row>
-    <row r="26" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C26" s="4" t="s">
+    <row r="26" spans="4:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="E26" t="s">
+      <c r="F26" t="s">
         <v>76</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>326</v>
       </c>
-      <c r="I26" t="s">
+      <c r="J26" t="s">
         <v>497</v>
       </c>
-      <c r="M26" t="s">
+      <c r="N26" t="s">
         <v>666</v>
       </c>
-      <c r="Q26" t="s">
+      <c r="R26" t="s">
         <v>735</v>
       </c>
-      <c r="S26" t="s">
+      <c r="T26" t="s">
         <v>787</v>
       </c>
     </row>
-    <row r="27" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C27" s="4" t="s">
+    <row r="27" spans="4:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E27" t="s">
+      <c r="F27" t="s">
         <v>77</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>327</v>
       </c>
-      <c r="I27" t="s">
+      <c r="J27" t="s">
         <v>498</v>
       </c>
-      <c r="M27" t="s">
+      <c r="N27" t="s">
         <v>667</v>
       </c>
-      <c r="Q27" t="s">
+      <c r="R27" t="s">
         <v>736</v>
       </c>
-      <c r="S27" t="s">
+      <c r="T27" t="s">
         <v>788</v>
       </c>
     </row>
-    <row r="28" spans="3:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C28" s="4" t="s">
+    <row r="28" spans="4:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E28" t="s">
+      <c r="F28" t="s">
         <v>78</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>328</v>
       </c>
-      <c r="I28" t="s">
+      <c r="J28" t="s">
         <v>499</v>
       </c>
-      <c r="M28" t="s">
+      <c r="N28" t="s">
         <v>668</v>
       </c>
-      <c r="Q28" t="s">
+      <c r="R28" t="s">
         <v>737</v>
       </c>
-      <c r="S28" t="s">
+      <c r="T28" t="s">
         <v>789</v>
       </c>
     </row>
-    <row r="29" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="E29" t="s">
+    <row r="29" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="F29" t="s">
         <v>79</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>329</v>
       </c>
-      <c r="I29" t="s">
+      <c r="J29" t="s">
         <v>500</v>
       </c>
-      <c r="M29" t="s">
+      <c r="N29" t="s">
         <v>669</v>
       </c>
-      <c r="Q29" t="s">
+      <c r="R29" t="s">
         <v>738</v>
       </c>
-      <c r="S29" t="s">
+      <c r="T29" t="s">
         <v>790</v>
       </c>
     </row>
-    <row r="30" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="E30" t="s">
+    <row r="30" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="F30" t="s">
         <v>80</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>330</v>
       </c>
-      <c r="I30" t="s">
+      <c r="J30" t="s">
         <v>501</v>
       </c>
-      <c r="M30" t="s">
+      <c r="N30" t="s">
         <v>670</v>
       </c>
-      <c r="Q30" t="s">
+      <c r="R30" t="s">
         <v>739</v>
       </c>
-      <c r="S30" t="s">
+      <c r="T30" t="s">
         <v>791</v>
       </c>
     </row>
-    <row r="31" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="E31" t="s">
+    <row r="31" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="F31" t="s">
         <v>81</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>331</v>
       </c>
-      <c r="I31" t="s">
+      <c r="J31" t="s">
         <v>502</v>
       </c>
-      <c r="M31" t="s">
+      <c r="N31" t="s">
         <v>671</v>
       </c>
-      <c r="Q31" t="s">
+      <c r="R31" t="s">
         <v>740</v>
       </c>
-      <c r="S31" t="s">
+      <c r="T31" t="s">
         <v>792</v>
       </c>
     </row>
-    <row r="32" spans="3:19" x14ac:dyDescent="0.25">
-      <c r="E32" t="s">
+    <row r="32" spans="4:20" x14ac:dyDescent="0.25">
+      <c r="F32" t="s">
         <v>82</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>332</v>
       </c>
-      <c r="I32" t="s">
+      <c r="J32" t="s">
         <v>503</v>
       </c>
-      <c r="M32" t="s">
+      <c r="N32" t="s">
         <v>672</v>
       </c>
-      <c r="Q32" t="s">
+      <c r="R32" t="s">
         <v>741</v>
       </c>
-      <c r="S32" t="s">
+      <c r="T32" t="s">
         <v>793</v>
       </c>
     </row>
-    <row r="33" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E33" t="s">
+    <row r="33" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F33" t="s">
         <v>83</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>333</v>
       </c>
-      <c r="I33" t="s">
+      <c r="J33" t="s">
         <v>504</v>
       </c>
-      <c r="M33" t="s">
+      <c r="N33" t="s">
         <v>673</v>
       </c>
-      <c r="Q33" t="s">
+      <c r="R33" t="s">
         <v>742</v>
       </c>
-      <c r="S33" t="s">
+      <c r="T33" t="s">
         <v>794</v>
       </c>
     </row>
-    <row r="34" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E34" t="s">
+    <row r="34" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F34" t="s">
         <v>84</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>334</v>
       </c>
-      <c r="I34" t="s">
+      <c r="J34" t="s">
         <v>505</v>
       </c>
-      <c r="M34" t="s">
+      <c r="N34" t="s">
         <v>674</v>
       </c>
-      <c r="Q34" t="s">
+      <c r="R34" t="s">
         <v>743</v>
       </c>
-      <c r="S34" t="s">
+      <c r="T34" t="s">
         <v>795</v>
       </c>
     </row>
-    <row r="35" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E35" t="s">
+    <row r="35" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F35" t="s">
         <v>85</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>335</v>
       </c>
-      <c r="I35" t="s">
+      <c r="J35" t="s">
         <v>506</v>
       </c>
-      <c r="M35" t="s">
+      <c r="N35" t="s">
         <v>675</v>
       </c>
-      <c r="Q35" t="s">
+      <c r="R35" t="s">
         <v>744</v>
       </c>
-      <c r="S35" t="s">
+      <c r="T35" t="s">
         <v>796</v>
       </c>
     </row>
-    <row r="36" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E36" t="s">
+    <row r="36" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F36" t="s">
         <v>86</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>336</v>
       </c>
-      <c r="I36" t="s">
+      <c r="J36" t="s">
         <v>507</v>
       </c>
-      <c r="M36" t="s">
+      <c r="N36" t="s">
         <v>676</v>
       </c>
-      <c r="Q36" t="s">
+      <c r="R36" t="s">
         <v>745</v>
       </c>
-      <c r="S36" t="s">
+      <c r="T36" t="s">
         <v>797</v>
       </c>
     </row>
-    <row r="37" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E37" t="s">
+    <row r="37" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F37" t="s">
         <v>87</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>337</v>
       </c>
-      <c r="I37" t="s">
+      <c r="J37" t="s">
         <v>508</v>
       </c>
-      <c r="M37" t="s">
+      <c r="N37" t="s">
         <v>677</v>
       </c>
-      <c r="Q37" t="s">
+      <c r="R37" t="s">
         <v>746</v>
       </c>
-      <c r="S37" t="s">
+      <c r="T37" t="s">
         <v>798</v>
       </c>
     </row>
-    <row r="38" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E38" t="s">
+    <row r="38" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F38" t="s">
         <v>88</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>338</v>
       </c>
-      <c r="I38" t="s">
+      <c r="J38" t="s">
         <v>509</v>
       </c>
-      <c r="M38" t="s">
+      <c r="N38" t="s">
         <v>678</v>
       </c>
-      <c r="Q38" t="s">
+      <c r="R38" t="s">
         <v>747</v>
       </c>
-      <c r="S38" t="s">
+      <c r="T38" t="s">
         <v>799</v>
       </c>
     </row>
-    <row r="39" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E39" t="s">
+    <row r="39" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F39" t="s">
         <v>89</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>339</v>
       </c>
-      <c r="I39" t="s">
+      <c r="J39" t="s">
         <v>510</v>
       </c>
-      <c r="M39" t="s">
+      <c r="N39" t="s">
         <v>679</v>
       </c>
-      <c r="Q39" t="s">
+      <c r="R39" t="s">
         <v>748</v>
       </c>
-      <c r="S39" t="s">
+      <c r="T39" t="s">
         <v>800</v>
       </c>
     </row>
-    <row r="40" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E40" t="s">
+    <row r="40" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F40" t="s">
         <v>90</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>340</v>
       </c>
-      <c r="I40" t="s">
+      <c r="J40" t="s">
         <v>511</v>
       </c>
-      <c r="M40" t="s">
+      <c r="N40" t="s">
         <v>680</v>
       </c>
-      <c r="Q40" t="s">
+      <c r="R40" t="s">
         <v>749</v>
       </c>
-      <c r="S40" t="s">
+      <c r="T40" t="s">
         <v>801</v>
       </c>
     </row>
-    <row r="41" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E41" t="s">
+    <row r="41" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F41" t="s">
         <v>91</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>341</v>
       </c>
-      <c r="I41" t="s">
+      <c r="J41" t="s">
         <v>512</v>
       </c>
-      <c r="M41" t="s">
+      <c r="N41" t="s">
         <v>681</v>
       </c>
-      <c r="Q41" t="s">
+      <c r="R41" t="s">
         <v>750</v>
       </c>
-      <c r="S41" t="s">
+      <c r="T41" t="s">
         <v>802</v>
       </c>
     </row>
-    <row r="42" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E42" t="s">
+    <row r="42" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F42" t="s">
         <v>92</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>342</v>
       </c>
-      <c r="I42" t="s">
+      <c r="J42" t="s">
         <v>513</v>
       </c>
-      <c r="Q42" t="s">
+      <c r="R42" t="s">
         <v>751</v>
       </c>
-      <c r="S42" t="s">
+      <c r="T42" t="s">
         <v>803</v>
       </c>
     </row>
-    <row r="43" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E43" t="s">
+    <row r="43" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F43" t="s">
         <v>93</v>
       </c>
-      <c r="G43" t="s">
+      <c r="H43" t="s">
         <v>343</v>
       </c>
-      <c r="I43" t="s">
+      <c r="J43" t="s">
         <v>514</v>
       </c>
-      <c r="Q43" t="s">
+      <c r="R43" t="s">
         <v>752</v>
       </c>
-      <c r="S43" t="s">
+      <c r="T43" t="s">
         <v>804</v>
       </c>
     </row>
-    <row r="44" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E44" t="s">
+    <row r="44" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F44" t="s">
         <v>94</v>
       </c>
-      <c r="G44" t="s">
+      <c r="H44" t="s">
         <v>344</v>
       </c>
-      <c r="I44" t="s">
+      <c r="J44" t="s">
         <v>515</v>
       </c>
-      <c r="Q44" t="s">
+      <c r="R44" t="s">
         <v>753</v>
       </c>
-      <c r="S44" t="s">
+      <c r="T44" t="s">
         <v>805</v>
       </c>
     </row>
-    <row r="45" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E45" t="s">
+    <row r="45" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F45" t="s">
         <v>95</v>
       </c>
-      <c r="G45" t="s">
+      <c r="H45" t="s">
         <v>345</v>
       </c>
-      <c r="I45" t="s">
+      <c r="J45" t="s">
         <v>516</v>
       </c>
-      <c r="Q45" t="s">
+      <c r="R45" t="s">
         <v>754</v>
       </c>
-      <c r="S45" t="s">
+      <c r="T45" t="s">
         <v>806</v>
       </c>
     </row>
-    <row r="46" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E46" t="s">
+    <row r="46" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F46" t="s">
         <v>96</v>
       </c>
-      <c r="G46" t="s">
+      <c r="H46" t="s">
         <v>346</v>
       </c>
-      <c r="I46" t="s">
+      <c r="J46" t="s">
         <v>517</v>
       </c>
-      <c r="Q46" t="s">
+      <c r="R46" t="s">
         <v>755</v>
       </c>
-      <c r="S46" t="s">
+      <c r="T46" t="s">
         <v>807</v>
       </c>
     </row>
-    <row r="47" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E47" t="s">
+    <row r="47" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F47" t="s">
         <v>97</v>
       </c>
-      <c r="G47" t="s">
+      <c r="H47" t="s">
         <v>347</v>
       </c>
-      <c r="I47" t="s">
+      <c r="J47" t="s">
         <v>518</v>
       </c>
-      <c r="Q47" t="s">
+      <c r="R47" t="s">
         <v>756</v>
       </c>
-      <c r="S47" t="s">
+      <c r="T47" t="s">
         <v>808</v>
       </c>
     </row>
-    <row r="48" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E48" t="s">
+    <row r="48" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F48" t="s">
         <v>98</v>
       </c>
-      <c r="G48" t="s">
+      <c r="H48" t="s">
         <v>348</v>
       </c>
-      <c r="I48" t="s">
+      <c r="J48" t="s">
         <v>519</v>
       </c>
-      <c r="Q48" t="s">
+      <c r="R48" t="s">
         <v>757</v>
       </c>
-      <c r="S48" t="s">
+      <c r="T48" t="s">
         <v>809</v>
       </c>
     </row>
-    <row r="49" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E49" t="s">
+    <row r="49" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F49" t="s">
         <v>99</v>
       </c>
-      <c r="G49" t="s">
+      <c r="H49" t="s">
         <v>349</v>
       </c>
-      <c r="I49" t="s">
+      <c r="J49" t="s">
         <v>520</v>
       </c>
-      <c r="Q49" t="s">
+      <c r="R49" t="s">
         <v>758</v>
       </c>
-      <c r="S49" t="s">
+      <c r="T49" t="s">
         <v>810</v>
       </c>
     </row>
-    <row r="50" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E50" t="s">
+    <row r="50" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F50" t="s">
         <v>100</v>
       </c>
-      <c r="G50" t="s">
+      <c r="H50" t="s">
         <v>350</v>
       </c>
-      <c r="I50" t="s">
+      <c r="J50" t="s">
         <v>521</v>
       </c>
-      <c r="Q50" t="s">
+      <c r="R50" t="s">
         <v>759</v>
       </c>
-      <c r="S50" t="s">
+      <c r="T50" t="s">
         <v>811</v>
       </c>
     </row>
-    <row r="51" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E51" t="s">
+    <row r="51" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F51" t="s">
         <v>101</v>
       </c>
-      <c r="G51" t="s">
+      <c r="H51" t="s">
         <v>351</v>
       </c>
-      <c r="I51" t="s">
+      <c r="J51" t="s">
         <v>522</v>
       </c>
-      <c r="Q51" t="s">
+      <c r="R51" t="s">
         <v>760</v>
       </c>
-      <c r="S51" t="s">
+      <c r="T51" t="s">
         <v>812</v>
       </c>
     </row>
-    <row r="52" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E52" t="s">
+    <row r="52" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F52" t="s">
         <v>102</v>
       </c>
-      <c r="G52" t="s">
+      <c r="H52" t="s">
         <v>352</v>
       </c>
-      <c r="I52" t="s">
+      <c r="J52" t="s">
         <v>523</v>
       </c>
-      <c r="Q52" t="s">
+      <c r="R52" t="s">
         <v>761</v>
       </c>
-      <c r="S52" t="s">
+      <c r="T52" t="s">
         <v>813</v>
       </c>
     </row>
-    <row r="53" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E53" t="s">
+    <row r="53" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F53" t="s">
         <v>103</v>
       </c>
-      <c r="G53" t="s">
+      <c r="H53" t="s">
         <v>353</v>
       </c>
-      <c r="I53" t="s">
+      <c r="J53" t="s">
         <v>524</v>
       </c>
-      <c r="S53" t="s">
+      <c r="T53" t="s">
         <v>814</v>
       </c>
     </row>
-    <row r="54" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E54" t="s">
+    <row r="54" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F54" t="s">
         <v>104</v>
       </c>
-      <c r="G54" t="s">
+      <c r="H54" t="s">
         <v>354</v>
       </c>
-      <c r="I54" t="s">
+      <c r="J54" t="s">
         <v>525</v>
       </c>
-      <c r="S54" t="s">
+      <c r="T54" t="s">
         <v>815</v>
       </c>
     </row>
-    <row r="55" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E55" t="s">
+    <row r="55" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F55" t="s">
         <v>105</v>
       </c>
-      <c r="G55" t="s">
+      <c r="H55" t="s">
         <v>355</v>
       </c>
-      <c r="I55" t="s">
+      <c r="J55" t="s">
         <v>526</v>
       </c>
-      <c r="S55" t="s">
+      <c r="T55" t="s">
         <v>816</v>
       </c>
     </row>
-    <row r="56" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E56" t="s">
+    <row r="56" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F56" t="s">
         <v>106</v>
       </c>
-      <c r="G56" t="s">
+      <c r="H56" t="s">
         <v>356</v>
       </c>
-      <c r="I56" t="s">
+      <c r="J56" t="s">
         <v>527</v>
       </c>
-      <c r="S56" t="s">
+      <c r="T56" t="s">
         <v>817</v>
       </c>
     </row>
-    <row r="57" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E57" t="s">
+    <row r="57" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F57" t="s">
         <v>107</v>
       </c>
-      <c r="G57" t="s">
+      <c r="H57" t="s">
         <v>357</v>
       </c>
-      <c r="I57" t="s">
+      <c r="J57" t="s">
         <v>528</v>
       </c>
-      <c r="S57" t="s">
+      <c r="T57" t="s">
         <v>818</v>
       </c>
     </row>
-    <row r="58" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E58" t="s">
+    <row r="58" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F58" t="s">
         <v>108</v>
       </c>
-      <c r="G58" t="s">
+      <c r="H58" t="s">
         <v>358</v>
       </c>
-      <c r="I58" t="s">
+      <c r="J58" t="s">
         <v>529</v>
       </c>
-      <c r="S58" t="s">
+      <c r="T58" t="s">
         <v>819</v>
       </c>
     </row>
-    <row r="59" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E59" t="s">
+    <row r="59" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F59" t="s">
         <v>109</v>
       </c>
-      <c r="G59" t="s">
+      <c r="H59" t="s">
         <v>359</v>
       </c>
-      <c r="I59" t="s">
+      <c r="J59" t="s">
         <v>530</v>
       </c>
-      <c r="S59" t="s">
+      <c r="T59" t="s">
         <v>820</v>
       </c>
     </row>
-    <row r="60" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E60" t="s">
+    <row r="60" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F60" t="s">
         <v>110</v>
       </c>
-      <c r="G60" t="s">
+      <c r="H60" t="s">
         <v>360</v>
       </c>
-      <c r="I60" t="s">
+      <c r="J60" t="s">
         <v>531</v>
       </c>
-      <c r="S60" t="s">
+      <c r="T60" t="s">
         <v>821</v>
       </c>
     </row>
-    <row r="61" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E61" t="s">
+    <row r="61" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F61" t="s">
         <v>111</v>
       </c>
-      <c r="G61" t="s">
+      <c r="H61" t="s">
         <v>361</v>
       </c>
-      <c r="I61" t="s">
+      <c r="J61" t="s">
         <v>532</v>
       </c>
-      <c r="S61" t="s">
+      <c r="T61" t="s">
         <v>822</v>
       </c>
     </row>
-    <row r="62" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E62" t="s">
+    <row r="62" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F62" t="s">
         <v>112</v>
       </c>
-      <c r="G62" t="s">
+      <c r="H62" t="s">
         <v>362</v>
       </c>
-      <c r="I62" t="s">
+      <c r="J62" t="s">
         <v>533</v>
       </c>
-      <c r="S62" t="s">
+      <c r="T62" t="s">
         <v>823</v>
       </c>
     </row>
-    <row r="63" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E63" t="s">
+    <row r="63" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F63" t="s">
         <v>113</v>
       </c>
-      <c r="G63" t="s">
+      <c r="H63" t="s">
         <v>363</v>
       </c>
-      <c r="I63" t="s">
+      <c r="J63" t="s">
         <v>534</v>
       </c>
-      <c r="S63" t="s">
+      <c r="T63" t="s">
         <v>824</v>
       </c>
     </row>
-    <row r="64" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E64" t="s">
+    <row r="64" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F64" t="s">
         <v>114</v>
       </c>
-      <c r="G64" t="s">
+      <c r="H64" t="s">
         <v>364</v>
       </c>
-      <c r="I64" t="s">
+      <c r="J64" t="s">
         <v>535</v>
       </c>
-      <c r="S64" t="s">
+      <c r="T64" t="s">
         <v>825</v>
       </c>
     </row>
-    <row r="65" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E65" t="s">
+    <row r="65" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F65" t="s">
         <v>115</v>
       </c>
-      <c r="G65" t="s">
+      <c r="H65" t="s">
         <v>365</v>
       </c>
-      <c r="I65" t="s">
+      <c r="J65" t="s">
         <v>536</v>
       </c>
-      <c r="S65" t="s">
+      <c r="T65" t="s">
         <v>826</v>
       </c>
     </row>
-    <row r="66" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E66" t="s">
+    <row r="66" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F66" t="s">
         <v>116</v>
       </c>
-      <c r="G66" t="s">
+      <c r="H66" t="s">
         <v>366</v>
       </c>
-      <c r="I66" t="s">
+      <c r="J66" t="s">
         <v>537</v>
       </c>
-      <c r="S66" t="s">
+      <c r="T66" t="s">
         <v>827</v>
       </c>
     </row>
-    <row r="67" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E67" t="s">
+    <row r="67" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F67" t="s">
         <v>117</v>
       </c>
-      <c r="G67" t="s">
+      <c r="H67" t="s">
         <v>367</v>
       </c>
-      <c r="I67" t="s">
+      <c r="J67" t="s">
         <v>538</v>
       </c>
-      <c r="S67" t="s">
+      <c r="T67" t="s">
         <v>828</v>
       </c>
     </row>
-    <row r="68" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E68" t="s">
+    <row r="68" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F68" t="s">
         <v>118</v>
       </c>
-      <c r="G68" t="s">
+      <c r="H68" t="s">
         <v>368</v>
       </c>
-      <c r="I68" t="s">
+      <c r="J68" t="s">
         <v>539</v>
       </c>
-      <c r="S68" t="s">
+      <c r="T68" t="s">
         <v>829</v>
       </c>
     </row>
-    <row r="69" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E69" t="s">
+    <row r="69" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F69" t="s">
         <v>119</v>
       </c>
-      <c r="G69" t="s">
+      <c r="H69" t="s">
         <v>369</v>
       </c>
-      <c r="I69" t="s">
+      <c r="J69" t="s">
         <v>540</v>
       </c>
-      <c r="S69" t="s">
+      <c r="T69" t="s">
         <v>830</v>
       </c>
     </row>
-    <row r="70" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E70" t="s">
+    <row r="70" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F70" t="s">
         <v>120</v>
       </c>
-      <c r="G70" t="s">
+      <c r="H70" t="s">
         <v>370</v>
       </c>
-      <c r="I70" t="s">
+      <c r="J70" t="s">
         <v>541</v>
       </c>
-      <c r="S70" t="s">
+      <c r="T70" t="s">
         <v>831</v>
       </c>
     </row>
-    <row r="71" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E71" t="s">
+    <row r="71" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F71" t="s">
         <v>121</v>
       </c>
-      <c r="G71" t="s">
+      <c r="H71" t="s">
         <v>371</v>
       </c>
-      <c r="I71" t="s">
+      <c r="J71" t="s">
         <v>542</v>
       </c>
-      <c r="S71" t="s">
+      <c r="T71" t="s">
         <v>832</v>
       </c>
     </row>
-    <row r="72" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E72" t="s">
+    <row r="72" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F72" t="s">
         <v>122</v>
       </c>
-      <c r="G72" t="s">
+      <c r="H72" t="s">
         <v>372</v>
       </c>
-      <c r="I72" t="s">
+      <c r="J72" t="s">
         <v>543</v>
       </c>
-      <c r="S72" t="s">
+      <c r="T72" t="s">
         <v>833</v>
       </c>
     </row>
-    <row r="73" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E73" t="s">
+    <row r="73" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F73" t="s">
         <v>123</v>
       </c>
-      <c r="G73" t="s">
+      <c r="H73" t="s">
         <v>373</v>
       </c>
-      <c r="I73" t="s">
+      <c r="J73" t="s">
         <v>544</v>
       </c>
-      <c r="S73" t="s">
+      <c r="T73" t="s">
         <v>834</v>
       </c>
     </row>
-    <row r="74" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E74" t="s">
+    <row r="74" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F74" t="s">
         <v>124</v>
       </c>
-      <c r="G74" t="s">
+      <c r="H74" t="s">
         <v>374</v>
       </c>
-      <c r="I74" t="s">
+      <c r="J74" t="s">
         <v>545</v>
       </c>
-      <c r="S74" t="s">
+      <c r="T74" t="s">
         <v>835</v>
       </c>
     </row>
-    <row r="75" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E75" t="s">
+    <row r="75" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F75" t="s">
         <v>125</v>
       </c>
-      <c r="G75" t="s">
+      <c r="H75" t="s">
         <v>375</v>
       </c>
-      <c r="I75" t="s">
+      <c r="J75" t="s">
         <v>546</v>
       </c>
-      <c r="S75" t="s">
+      <c r="T75" t="s">
         <v>836</v>
       </c>
     </row>
-    <row r="76" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E76" t="s">
+    <row r="76" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F76" t="s">
         <v>126</v>
       </c>
-      <c r="G76" t="s">
+      <c r="H76" t="s">
         <v>376</v>
       </c>
-      <c r="I76" t="s">
+      <c r="J76" t="s">
         <v>547</v>
       </c>
-      <c r="S76" t="s">
+      <c r="T76" t="s">
         <v>837</v>
       </c>
     </row>
-    <row r="77" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E77" t="s">
+    <row r="77" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F77" t="s">
         <v>127</v>
       </c>
-      <c r="G77" t="s">
+      <c r="H77" t="s">
         <v>377</v>
       </c>
-      <c r="I77" t="s">
+      <c r="J77" t="s">
         <v>548</v>
       </c>
-      <c r="S77" t="s">
+      <c r="T77" t="s">
         <v>838</v>
       </c>
     </row>
-    <row r="78" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E78" t="s">
+    <row r="78" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F78" t="s">
         <v>128</v>
       </c>
-      <c r="G78" t="s">
+      <c r="H78" t="s">
         <v>378</v>
       </c>
-      <c r="I78" t="s">
+      <c r="J78" t="s">
         <v>549</v>
       </c>
-      <c r="S78" t="s">
+      <c r="T78" t="s">
         <v>839</v>
       </c>
     </row>
-    <row r="79" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E79" t="s">
+    <row r="79" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F79" t="s">
         <v>129</v>
       </c>
-      <c r="G79" t="s">
+      <c r="H79" t="s">
         <v>379</v>
       </c>
-      <c r="I79" t="s">
+      <c r="J79" t="s">
         <v>550</v>
       </c>
-      <c r="S79" t="s">
+      <c r="T79" t="s">
         <v>840</v>
       </c>
     </row>
-    <row r="80" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E80" t="s">
+    <row r="80" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F80" t="s">
         <v>130</v>
       </c>
-      <c r="G80" t="s">
+      <c r="H80" t="s">
         <v>380</v>
       </c>
-      <c r="I80" t="s">
+      <c r="J80" t="s">
         <v>551</v>
       </c>
-      <c r="S80" t="s">
+      <c r="T80" t="s">
         <v>841</v>
       </c>
     </row>
-    <row r="81" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E81" t="s">
+    <row r="81" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F81" t="s">
         <v>131</v>
       </c>
-      <c r="G81" t="s">
+      <c r="H81" t="s">
         <v>381</v>
       </c>
-      <c r="I81" t="s">
+      <c r="J81" t="s">
         <v>552</v>
       </c>
-      <c r="S81" t="s">
+      <c r="T81" t="s">
         <v>842</v>
       </c>
     </row>
-    <row r="82" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E82" t="s">
+    <row r="82" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F82" t="s">
         <v>132</v>
       </c>
-      <c r="G82" t="s">
+      <c r="H82" t="s">
         <v>382</v>
       </c>
-      <c r="I82" t="s">
+      <c r="J82" t="s">
         <v>553</v>
       </c>
-      <c r="S82" t="s">
+      <c r="T82" t="s">
         <v>843</v>
       </c>
     </row>
-    <row r="83" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E83" t="s">
+    <row r="83" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F83" t="s">
         <v>133</v>
       </c>
-      <c r="G83" t="s">
+      <c r="H83" t="s">
         <v>383</v>
       </c>
-      <c r="I83" t="s">
+      <c r="J83" t="s">
         <v>554</v>
       </c>
-      <c r="S83" t="s">
+      <c r="T83" t="s">
         <v>844</v>
       </c>
     </row>
-    <row r="84" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E84" t="s">
+    <row r="84" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F84" t="s">
         <v>134</v>
       </c>
-      <c r="G84" t="s">
+      <c r="H84" t="s">
         <v>384</v>
       </c>
-      <c r="I84" t="s">
+      <c r="J84" t="s">
         <v>555</v>
       </c>
-      <c r="S84" t="s">
+      <c r="T84" t="s">
         <v>845</v>
       </c>
     </row>
-    <row r="85" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E85" t="s">
+    <row r="85" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F85" t="s">
         <v>135</v>
       </c>
-      <c r="G85" t="s">
+      <c r="H85" t="s">
         <v>385</v>
       </c>
-      <c r="I85" t="s">
+      <c r="J85" t="s">
         <v>556</v>
       </c>
-      <c r="S85" t="s">
+      <c r="T85" t="s">
         <v>846</v>
       </c>
     </row>
-    <row r="86" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E86" t="s">
+    <row r="86" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F86" t="s">
         <v>136</v>
       </c>
-      <c r="G86" t="s">
+      <c r="H86" t="s">
         <v>386</v>
       </c>
-      <c r="I86" t="s">
+      <c r="J86" t="s">
         <v>557</v>
       </c>
-      <c r="S86" t="s">
+      <c r="T86" t="s">
         <v>847</v>
       </c>
     </row>
-    <row r="87" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E87" t="s">
+    <row r="87" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F87" t="s">
         <v>137</v>
       </c>
-      <c r="G87" t="s">
+      <c r="H87" t="s">
         <v>387</v>
       </c>
-      <c r="I87" t="s">
+      <c r="J87" t="s">
         <v>558</v>
       </c>
-      <c r="S87" t="s">
+      <c r="T87" t="s">
         <v>848</v>
       </c>
     </row>
-    <row r="88" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E88" t="s">
+    <row r="88" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F88" t="s">
         <v>138</v>
       </c>
-      <c r="G88" t="s">
+      <c r="H88" t="s">
         <v>388</v>
       </c>
-      <c r="I88" t="s">
+      <c r="J88" t="s">
         <v>559</v>
       </c>
-      <c r="S88" t="s">
+      <c r="T88" t="s">
         <v>849</v>
       </c>
     </row>
-    <row r="89" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E89" t="s">
+    <row r="89" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F89" t="s">
         <v>139</v>
       </c>
-      <c r="G89" t="s">
+      <c r="H89" t="s">
         <v>389</v>
       </c>
-      <c r="I89" t="s">
+      <c r="J89" t="s">
         <v>560</v>
       </c>
-      <c r="S89" t="s">
+      <c r="T89" t="s">
         <v>850</v>
       </c>
     </row>
-    <row r="90" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E90" t="s">
+    <row r="90" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F90" t="s">
         <v>140</v>
       </c>
-      <c r="G90" t="s">
+      <c r="H90" t="s">
         <v>390</v>
       </c>
-      <c r="I90" t="s">
+      <c r="J90" t="s">
         <v>561</v>
       </c>
-      <c r="S90" t="s">
+      <c r="T90" t="s">
         <v>851</v>
       </c>
     </row>
-    <row r="91" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E91" t="s">
+    <row r="91" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F91" t="s">
         <v>141</v>
       </c>
-      <c r="G91" t="s">
+      <c r="H91" t="s">
         <v>391</v>
       </c>
-      <c r="I91" t="s">
+      <c r="J91" t="s">
         <v>562</v>
       </c>
-      <c r="S91" t="s">
+      <c r="T91" t="s">
         <v>852</v>
       </c>
     </row>
-    <row r="92" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E92" t="s">
+    <row r="92" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F92" t="s">
         <v>142</v>
       </c>
-      <c r="G92" t="s">
+      <c r="H92" t="s">
         <v>392</v>
       </c>
-      <c r="I92" t="s">
+      <c r="J92" t="s">
         <v>563</v>
       </c>
-      <c r="S92" t="s">
+      <c r="T92" t="s">
         <v>853</v>
       </c>
     </row>
-    <row r="93" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E93" t="s">
+    <row r="93" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F93" t="s">
         <v>143</v>
       </c>
-      <c r="G93" t="s">
+      <c r="H93" t="s">
         <v>393</v>
       </c>
-      <c r="I93" t="s">
+      <c r="J93" t="s">
         <v>564</v>
       </c>
-      <c r="S93" t="s">
+      <c r="T93" t="s">
         <v>854</v>
       </c>
     </row>
-    <row r="94" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E94" t="s">
+    <row r="94" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F94" t="s">
         <v>144</v>
       </c>
-      <c r="G94" t="s">
+      <c r="H94" t="s">
         <v>394</v>
       </c>
-      <c r="I94" t="s">
+      <c r="J94" t="s">
         <v>565</v>
       </c>
-      <c r="S94" t="s">
+      <c r="T94" t="s">
         <v>855</v>
       </c>
     </row>
-    <row r="95" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E95" t="s">
+    <row r="95" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F95" t="s">
         <v>145</v>
       </c>
-      <c r="G95" t="s">
+      <c r="H95" t="s">
         <v>395</v>
       </c>
-      <c r="I95" t="s">
+      <c r="J95" t="s">
         <v>566</v>
       </c>
-      <c r="S95" t="s">
+      <c r="T95" t="s">
         <v>856</v>
       </c>
     </row>
-    <row r="96" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E96" t="s">
+    <row r="96" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F96" t="s">
         <v>146</v>
       </c>
-      <c r="G96" t="s">
+      <c r="H96" t="s">
         <v>396</v>
       </c>
-      <c r="I96" t="s">
+      <c r="J96" t="s">
         <v>567</v>
       </c>
-      <c r="S96" t="s">
+      <c r="T96" t="s">
         <v>857</v>
       </c>
     </row>
-    <row r="97" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E97" t="s">
+    <row r="97" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F97" t="s">
         <v>147</v>
       </c>
-      <c r="G97" t="s">
+      <c r="H97" t="s">
         <v>397</v>
       </c>
-      <c r="I97" t="s">
+      <c r="J97" t="s">
         <v>568</v>
       </c>
-      <c r="S97" t="s">
+      <c r="T97" t="s">
         <v>858</v>
       </c>
     </row>
-    <row r="98" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E98" t="s">
+    <row r="98" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F98" t="s">
         <v>148</v>
       </c>
-      <c r="G98" t="s">
+      <c r="H98" t="s">
         <v>398</v>
       </c>
-      <c r="I98" t="s">
+      <c r="J98" t="s">
         <v>569</v>
       </c>
-      <c r="S98" t="s">
+      <c r="T98" t="s">
         <v>859</v>
       </c>
     </row>
-    <row r="99" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E99" t="s">
+    <row r="99" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F99" t="s">
         <v>149</v>
       </c>
-      <c r="G99" t="s">
+      <c r="H99" t="s">
         <v>399</v>
       </c>
-      <c r="I99" t="s">
+      <c r="J99" t="s">
         <v>570</v>
       </c>
-      <c r="S99" t="s">
+      <c r="T99" t="s">
         <v>860</v>
       </c>
     </row>
-    <row r="100" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E100" t="s">
+    <row r="100" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F100" t="s">
         <v>150</v>
       </c>
-      <c r="G100" t="s">
+      <c r="H100" t="s">
         <v>400</v>
       </c>
-      <c r="I100" t="s">
+      <c r="J100" t="s">
         <v>571</v>
       </c>
-      <c r="S100" t="s">
+      <c r="T100" t="s">
         <v>861</v>
       </c>
     </row>
-    <row r="101" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E101" t="s">
+    <row r="101" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F101" t="s">
         <v>151</v>
       </c>
-      <c r="G101" t="s">
+      <c r="H101" t="s">
         <v>401</v>
       </c>
-      <c r="I101" t="s">
+      <c r="J101" t="s">
         <v>572</v>
       </c>
-      <c r="S101" t="s">
+      <c r="T101" t="s">
         <v>862</v>
       </c>
     </row>
-    <row r="102" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E102" t="s">
+    <row r="102" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F102" t="s">
         <v>152</v>
       </c>
-      <c r="G102" t="s">
+      <c r="H102" t="s">
         <v>402</v>
       </c>
-      <c r="I102" t="s">
+      <c r="J102" t="s">
         <v>573</v>
       </c>
-      <c r="S102" t="s">
+      <c r="T102" t="s">
         <v>863</v>
       </c>
     </row>
-    <row r="103" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E103" t="s">
+    <row r="103" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F103" t="s">
         <v>153</v>
       </c>
-      <c r="G103" t="s">
+      <c r="H103" t="s">
         <v>403</v>
       </c>
-      <c r="I103" t="s">
+      <c r="J103" t="s">
         <v>574</v>
       </c>
-      <c r="S103" t="s">
+      <c r="T103" t="s">
         <v>864</v>
       </c>
     </row>
-    <row r="104" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E104" t="s">
+    <row r="104" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F104" t="s">
         <v>154</v>
       </c>
-      <c r="G104" t="s">
+      <c r="H104" t="s">
         <v>404</v>
       </c>
-      <c r="I104" t="s">
+      <c r="J104" t="s">
         <v>575</v>
       </c>
-      <c r="S104" t="s">
+      <c r="T104" t="s">
         <v>865</v>
       </c>
     </row>
-    <row r="105" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E105" t="s">
+    <row r="105" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F105" t="s">
         <v>155</v>
       </c>
-      <c r="G105" t="s">
+      <c r="H105" t="s">
         <v>405</v>
       </c>
-      <c r="I105" t="s">
+      <c r="J105" t="s">
         <v>576</v>
       </c>
-      <c r="S105" t="s">
+      <c r="T105" t="s">
         <v>866</v>
       </c>
     </row>
-    <row r="106" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E106" t="s">
+    <row r="106" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F106" t="s">
         <v>156</v>
       </c>
-      <c r="G106" t="s">
+      <c r="H106" t="s">
         <v>406</v>
       </c>
-      <c r="I106" t="s">
+      <c r="J106" t="s">
         <v>577</v>
       </c>
-      <c r="S106" t="s">
+      <c r="T106" t="s">
         <v>867</v>
       </c>
     </row>
-    <row r="107" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E107" t="s">
+    <row r="107" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F107" t="s">
         <v>157</v>
       </c>
-      <c r="G107" t="s">
+      <c r="H107" t="s">
         <v>407</v>
       </c>
-      <c r="I107" t="s">
+      <c r="J107" t="s">
         <v>578</v>
       </c>
-      <c r="S107" t="s">
+      <c r="T107" t="s">
         <v>868</v>
       </c>
     </row>
-    <row r="108" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E108" t="s">
+    <row r="108" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F108" t="s">
         <v>158</v>
       </c>
-      <c r="G108" t="s">
+      <c r="H108" t="s">
         <v>408</v>
       </c>
-      <c r="I108" t="s">
+      <c r="J108" t="s">
         <v>579</v>
       </c>
-      <c r="S108" t="s">
+      <c r="T108" t="s">
         <v>869</v>
       </c>
     </row>
-    <row r="109" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E109" t="s">
+    <row r="109" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F109" t="s">
         <v>159</v>
       </c>
-      <c r="G109" t="s">
+      <c r="H109" t="s">
         <v>409</v>
       </c>
-      <c r="I109" t="s">
+      <c r="J109" t="s">
         <v>580</v>
       </c>
-      <c r="S109" t="s">
+      <c r="T109" t="s">
         <v>870</v>
       </c>
     </row>
-    <row r="110" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E110" t="s">
+    <row r="110" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F110" t="s">
         <v>160</v>
       </c>
-      <c r="G110" t="s">
+      <c r="H110" t="s">
         <v>410</v>
       </c>
-      <c r="I110" t="s">
+      <c r="J110" t="s">
         <v>581</v>
       </c>
-      <c r="S110" t="s">
+      <c r="T110" t="s">
         <v>871</v>
       </c>
     </row>
-    <row r="111" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E111" t="s">
+    <row r="111" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F111" t="s">
         <v>161</v>
       </c>
-      <c r="G111" t="s">
+      <c r="H111" t="s">
         <v>411</v>
       </c>
-      <c r="I111" t="s">
+      <c r="J111" t="s">
         <v>582</v>
       </c>
-      <c r="S111" t="s">
+      <c r="T111" t="s">
         <v>872</v>
       </c>
     </row>
-    <row r="112" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E112" t="s">
+    <row r="112" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F112" t="s">
         <v>162</v>
       </c>
-      <c r="G112" t="s">
+      <c r="H112" t="s">
         <v>412</v>
       </c>
-      <c r="I112" t="s">
+      <c r="J112" t="s">
         <v>583</v>
       </c>
-      <c r="S112" t="s">
+      <c r="T112" t="s">
         <v>873</v>
       </c>
     </row>
-    <row r="113" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E113" t="s">
+    <row r="113" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F113" t="s">
         <v>163</v>
       </c>
-      <c r="G113" t="s">
+      <c r="H113" t="s">
         <v>413</v>
       </c>
-      <c r="I113" t="s">
+      <c r="J113" t="s">
         <v>584</v>
       </c>
-      <c r="S113" t="s">
+      <c r="T113" t="s">
         <v>874</v>
       </c>
     </row>
-    <row r="114" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E114" t="s">
+    <row r="114" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F114" t="s">
         <v>164</v>
       </c>
-      <c r="G114" t="s">
+      <c r="H114" t="s">
         <v>414</v>
       </c>
-      <c r="I114" t="s">
+      <c r="J114" t="s">
         <v>585</v>
       </c>
-      <c r="S114" t="s">
+      <c r="T114" t="s">
         <v>875</v>
       </c>
     </row>
-    <row r="115" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E115" t="s">
+    <row r="115" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F115" t="s">
         <v>165</v>
       </c>
-      <c r="G115" t="s">
+      <c r="H115" t="s">
         <v>415</v>
       </c>
-      <c r="I115" t="s">
+      <c r="J115" t="s">
         <v>586</v>
       </c>
-      <c r="S115" t="s">
+      <c r="T115" t="s">
         <v>876</v>
       </c>
     </row>
-    <row r="116" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E116" t="s">
+    <row r="116" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F116" t="s">
         <v>166</v>
       </c>
-      <c r="G116" t="s">
+      <c r="H116" t="s">
         <v>416</v>
       </c>
-      <c r="I116" t="s">
+      <c r="J116" t="s">
         <v>587</v>
       </c>
-      <c r="S116" t="s">
+      <c r="T116" t="s">
         <v>877</v>
       </c>
     </row>
-    <row r="117" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E117" t="s">
+    <row r="117" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F117" t="s">
         <v>167</v>
       </c>
-      <c r="G117" t="s">
+      <c r="H117" t="s">
         <v>417</v>
       </c>
-      <c r="I117" t="s">
+      <c r="J117" t="s">
         <v>588</v>
       </c>
-      <c r="S117" t="s">
+      <c r="T117" t="s">
         <v>878</v>
       </c>
     </row>
-    <row r="118" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E118" t="s">
+    <row r="118" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F118" t="s">
         <v>168</v>
       </c>
-      <c r="G118" t="s">
+      <c r="H118" t="s">
         <v>418</v>
       </c>
-      <c r="I118" t="s">
+      <c r="J118" t="s">
         <v>589</v>
       </c>
-      <c r="S118" t="s">
+      <c r="T118" t="s">
         <v>879</v>
       </c>
     </row>
-    <row r="119" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E119" t="s">
+    <row r="119" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F119" t="s">
         <v>169</v>
       </c>
-      <c r="G119" t="s">
+      <c r="H119" t="s">
         <v>419</v>
       </c>
-      <c r="I119" t="s">
+      <c r="J119" t="s">
         <v>590</v>
       </c>
-      <c r="S119" t="s">
+      <c r="T119" t="s">
         <v>880</v>
       </c>
     </row>
-    <row r="120" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E120" t="s">
+    <row r="120" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F120" t="s">
         <v>170</v>
       </c>
-      <c r="G120" t="s">
+      <c r="H120" t="s">
         <v>420</v>
       </c>
-      <c r="I120" t="s">
+      <c r="J120" t="s">
         <v>591</v>
       </c>
-      <c r="S120" t="s">
+      <c r="T120" t="s">
         <v>881</v>
       </c>
     </row>
-    <row r="121" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E121" t="s">
+    <row r="121" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F121" t="s">
         <v>171</v>
       </c>
-      <c r="G121" t="s">
+      <c r="H121" t="s">
         <v>421</v>
       </c>
-      <c r="I121" t="s">
+      <c r="J121" t="s">
         <v>592</v>
       </c>
-      <c r="S121" t="s">
+      <c r="T121" t="s">
         <v>882</v>
       </c>
     </row>
-    <row r="122" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E122" t="s">
+    <row r="122" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F122" t="s">
         <v>172</v>
       </c>
-      <c r="G122" t="s">
+      <c r="H122" t="s">
         <v>422</v>
       </c>
-      <c r="I122" t="s">
+      <c r="J122" t="s">
         <v>593</v>
       </c>
-      <c r="S122" t="s">
+      <c r="T122" t="s">
         <v>883</v>
       </c>
     </row>
-    <row r="123" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E123" t="s">
+    <row r="123" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F123" t="s">
         <v>173</v>
       </c>
-      <c r="G123" t="s">
+      <c r="H123" t="s">
         <v>423</v>
       </c>
-      <c r="I123" t="s">
+      <c r="J123" t="s">
         <v>594</v>
       </c>
-      <c r="S123" t="s">
+      <c r="T123" t="s">
         <v>884</v>
       </c>
     </row>
-    <row r="124" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E124" t="s">
+    <row r="124" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F124" t="s">
         <v>174</v>
       </c>
-      <c r="G124" t="s">
+      <c r="H124" t="s">
         <v>424</v>
       </c>
-      <c r="I124" t="s">
+      <c r="J124" t="s">
         <v>595</v>
       </c>
-      <c r="S124" t="s">
+      <c r="T124" t="s">
         <v>885</v>
       </c>
     </row>
-    <row r="125" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E125" t="s">
+    <row r="125" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F125" t="s">
         <v>175</v>
       </c>
-      <c r="G125" t="s">
+      <c r="H125" t="s">
         <v>425</v>
       </c>
-      <c r="I125" t="s">
+      <c r="J125" t="s">
         <v>596</v>
       </c>
-      <c r="S125" t="s">
+      <c r="T125" t="s">
         <v>886</v>
       </c>
     </row>
-    <row r="126" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E126" t="s">
+    <row r="126" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F126" t="s">
         <v>176</v>
       </c>
-      <c r="G126" t="s">
+      <c r="H126" t="s">
         <v>426</v>
       </c>
-      <c r="I126" t="s">
+      <c r="J126" t="s">
         <v>597</v>
       </c>
-      <c r="S126" t="s">
+      <c r="T126" t="s">
         <v>887</v>
       </c>
     </row>
-    <row r="127" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E127" t="s">
+    <row r="127" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F127" t="s">
         <v>177</v>
       </c>
-      <c r="G127" t="s">
+      <c r="H127" t="s">
         <v>427</v>
       </c>
-      <c r="I127" t="s">
+      <c r="J127" t="s">
         <v>598</v>
       </c>
-      <c r="S127" t="s">
+      <c r="T127" t="s">
         <v>888</v>
       </c>
     </row>
-    <row r="128" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E128" t="s">
+    <row r="128" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F128" t="s">
         <v>178</v>
       </c>
-      <c r="G128" t="s">
+      <c r="H128" t="s">
         <v>428</v>
       </c>
-      <c r="I128" t="s">
+      <c r="J128" t="s">
         <v>599</v>
       </c>
-      <c r="S128" t="s">
+      <c r="T128" t="s">
         <v>889</v>
       </c>
     </row>
-    <row r="129" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E129" t="s">
+    <row r="129" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F129" t="s">
         <v>179</v>
       </c>
-      <c r="G129" t="s">
+      <c r="H129" t="s">
         <v>429</v>
       </c>
-      <c r="I129" t="s">
+      <c r="J129" t="s">
         <v>600</v>
       </c>
-      <c r="S129" t="s">
+      <c r="T129" t="s">
         <v>890</v>
       </c>
     </row>
-    <row r="130" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E130" t="s">
+    <row r="130" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F130" t="s">
         <v>180</v>
       </c>
-      <c r="G130" t="s">
+      <c r="H130" t="s">
         <v>430</v>
       </c>
-      <c r="I130" t="s">
+      <c r="J130" t="s">
         <v>601</v>
       </c>
-      <c r="S130" t="s">
+      <c r="T130" t="s">
         <v>891</v>
       </c>
     </row>
-    <row r="131" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E131" t="s">
+    <row r="131" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F131" t="s">
         <v>181</v>
       </c>
-      <c r="G131" t="s">
+      <c r="H131" t="s">
         <v>431</v>
       </c>
-      <c r="I131" t="s">
+      <c r="J131" t="s">
         <v>602</v>
       </c>
-      <c r="S131" t="s">
+      <c r="T131" t="s">
         <v>892</v>
       </c>
     </row>
-    <row r="132" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E132" t="s">
+    <row r="132" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F132" t="s">
         <v>182</v>
       </c>
-      <c r="G132" t="s">
+      <c r="H132" t="s">
         <v>432</v>
       </c>
-      <c r="I132" t="s">
+      <c r="J132" t="s">
         <v>603</v>
       </c>
-      <c r="S132" t="s">
+      <c r="T132" t="s">
         <v>893</v>
       </c>
     </row>
-    <row r="133" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E133" t="s">
+    <row r="133" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F133" t="s">
         <v>183</v>
       </c>
-      <c r="G133" t="s">
+      <c r="H133" t="s">
         <v>433</v>
       </c>
-      <c r="I133" t="s">
+      <c r="J133" t="s">
         <v>604</v>
       </c>
-      <c r="S133" t="s">
+      <c r="T133" t="s">
         <v>894</v>
       </c>
     </row>
-    <row r="134" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E134" t="s">
+    <row r="134" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F134" t="s">
         <v>184</v>
       </c>
-      <c r="G134" t="s">
+      <c r="H134" t="s">
         <v>434</v>
       </c>
-      <c r="I134" t="s">
+      <c r="J134" t="s">
         <v>605</v>
       </c>
-      <c r="S134" t="s">
+      <c r="T134" t="s">
         <v>895</v>
       </c>
     </row>
-    <row r="135" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E135" t="s">
+    <row r="135" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F135" t="s">
         <v>185</v>
       </c>
-      <c r="G135" t="s">
+      <c r="H135" t="s">
         <v>435</v>
       </c>
-      <c r="I135" t="s">
+      <c r="J135" t="s">
         <v>606</v>
       </c>
-      <c r="S135" t="s">
+      <c r="T135" t="s">
         <v>896</v>
       </c>
     </row>
-    <row r="136" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E136" t="s">
+    <row r="136" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F136" t="s">
         <v>186</v>
       </c>
-      <c r="G136" t="s">
+      <c r="H136" t="s">
         <v>436</v>
       </c>
-      <c r="I136" t="s">
+      <c r="J136" t="s">
         <v>607</v>
       </c>
-      <c r="S136" t="s">
+      <c r="T136" t="s">
         <v>897</v>
       </c>
     </row>
-    <row r="137" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E137" t="s">
+    <row r="137" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F137" t="s">
         <v>187</v>
       </c>
-      <c r="G137" t="s">
+      <c r="H137" t="s">
         <v>437</v>
       </c>
-      <c r="I137" t="s">
+      <c r="J137" t="s">
         <v>608</v>
       </c>
-      <c r="S137" t="s">
+      <c r="T137" t="s">
         <v>898</v>
       </c>
     </row>
-    <row r="138" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E138" t="s">
+    <row r="138" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F138" t="s">
         <v>188</v>
       </c>
-      <c r="G138" t="s">
+      <c r="H138" t="s">
         <v>438</v>
       </c>
-      <c r="S138" t="s">
+      <c r="T138" t="s">
         <v>899</v>
       </c>
     </row>
-    <row r="139" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E139" t="s">
+    <row r="139" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F139" t="s">
         <v>189</v>
       </c>
-      <c r="G139" t="s">
+      <c r="H139" t="s">
         <v>439</v>
       </c>
-      <c r="S139" t="s">
+      <c r="T139" t="s">
         <v>900</v>
       </c>
     </row>
-    <row r="140" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E140" t="s">
+    <row r="140" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F140" t="s">
         <v>190</v>
       </c>
-      <c r="G140" t="s">
+      <c r="H140" t="s">
         <v>440</v>
       </c>
-      <c r="S140" t="s">
+      <c r="T140" t="s">
         <v>901</v>
       </c>
     </row>
-    <row r="141" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E141" t="s">
+    <row r="141" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F141" t="s">
         <v>191</v>
       </c>
-      <c r="G141" t="s">
+      <c r="H141" t="s">
         <v>441</v>
       </c>
-      <c r="S141" t="s">
+      <c r="T141" t="s">
         <v>902</v>
       </c>
     </row>
-    <row r="142" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E142" t="s">
+    <row r="142" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F142" t="s">
         <v>192</v>
       </c>
-      <c r="G142" t="s">
+      <c r="H142" t="s">
         <v>442</v>
       </c>
-      <c r="S142" t="s">
+      <c r="T142" t="s">
         <v>903</v>
       </c>
     </row>
-    <row r="143" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E143" t="s">
+    <row r="143" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F143" t="s">
         <v>193</v>
       </c>
-      <c r="G143" t="s">
+      <c r="H143" t="s">
         <v>443</v>
       </c>
-      <c r="S143" t="s">
+      <c r="T143" t="s">
         <v>904</v>
       </c>
     </row>
-    <row r="144" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E144" t="s">
+    <row r="144" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F144" t="s">
         <v>194</v>
       </c>
-      <c r="G144" t="s">
+      <c r="H144" t="s">
         <v>444</v>
       </c>
-      <c r="S144" t="s">
+      <c r="T144" t="s">
         <v>905</v>
       </c>
     </row>
-    <row r="145" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E145" t="s">
+    <row r="145" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F145" t="s">
         <v>195</v>
       </c>
-      <c r="G145" t="s">
+      <c r="H145" t="s">
         <v>445</v>
       </c>
-      <c r="S145" t="s">
+      <c r="T145" t="s">
         <v>906</v>
       </c>
     </row>
-    <row r="146" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E146" t="s">
+    <row r="146" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F146" t="s">
         <v>196</v>
       </c>
-      <c r="G146" t="s">
+      <c r="H146" t="s">
         <v>446</v>
       </c>
-      <c r="S146" t="s">
+      <c r="T146" t="s">
         <v>907</v>
       </c>
     </row>
-    <row r="147" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E147" t="s">
+    <row r="147" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F147" t="s">
         <v>197</v>
       </c>
-      <c r="G147" t="s">
+      <c r="H147" t="s">
         <v>447</v>
       </c>
-      <c r="S147" t="s">
+      <c r="T147" t="s">
         <v>908</v>
       </c>
     </row>
-    <row r="148" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E148" t="s">
+    <row r="148" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F148" t="s">
         <v>198</v>
       </c>
-      <c r="G148" t="s">
+      <c r="H148" t="s">
         <v>448</v>
       </c>
-      <c r="S148" t="s">
+      <c r="T148" t="s">
         <v>909</v>
       </c>
     </row>
-    <row r="149" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E149" t="s">
+    <row r="149" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F149" t="s">
         <v>199</v>
       </c>
-      <c r="G149" t="s">
+      <c r="H149" t="s">
         <v>449</v>
       </c>
-      <c r="S149" t="s">
+      <c r="T149" t="s">
         <v>910</v>
       </c>
     </row>
-    <row r="150" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E150" t="s">
+    <row r="150" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F150" t="s">
         <v>200</v>
       </c>
-      <c r="G150" t="s">
+      <c r="H150" t="s">
         <v>450</v>
       </c>
-      <c r="S150" t="s">
+      <c r="T150" t="s">
         <v>911</v>
       </c>
     </row>
-    <row r="151" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E151" t="s">
+    <row r="151" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F151" t="s">
         <v>201</v>
       </c>
-      <c r="G151" t="s">
+      <c r="H151" t="s">
         <v>451</v>
       </c>
-      <c r="S151" t="s">
+      <c r="T151" t="s">
         <v>912</v>
       </c>
     </row>
-    <row r="152" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E152" t="s">
+    <row r="152" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F152" t="s">
         <v>202</v>
       </c>
-      <c r="G152" t="s">
+      <c r="H152" t="s">
         <v>452</v>
       </c>
-      <c r="S152" t="s">
+      <c r="T152" t="s">
         <v>913</v>
       </c>
     </row>
-    <row r="153" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E153" t="s">
+    <row r="153" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F153" t="s">
         <v>203</v>
       </c>
-      <c r="G153" t="s">
+      <c r="H153" t="s">
         <v>453</v>
       </c>
-      <c r="S153" t="s">
+      <c r="T153" t="s">
         <v>914</v>
       </c>
     </row>
-    <row r="154" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E154" t="s">
+    <row r="154" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F154" t="s">
         <v>204</v>
       </c>
-      <c r="G154" t="s">
+      <c r="H154" t="s">
         <v>454</v>
       </c>
-      <c r="S154" t="s">
+      <c r="T154" t="s">
         <v>915</v>
       </c>
     </row>
-    <row r="155" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E155" t="s">
+    <row r="155" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F155" t="s">
         <v>205</v>
       </c>
-      <c r="G155" t="s">
+      <c r="H155" t="s">
         <v>455</v>
       </c>
-      <c r="S155" t="s">
+      <c r="T155" t="s">
         <v>916</v>
       </c>
     </row>
-    <row r="156" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E156" t="s">
+    <row r="156" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F156" t="s">
         <v>206</v>
       </c>
-      <c r="G156" t="s">
+      <c r="H156" t="s">
         <v>456</v>
       </c>
-      <c r="S156" t="s">
+      <c r="T156" t="s">
         <v>917</v>
       </c>
     </row>
-    <row r="157" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E157" t="s">
+    <row r="157" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F157" t="s">
         <v>207</v>
       </c>
-      <c r="G157" t="s">
+      <c r="H157" t="s">
         <v>457</v>
       </c>
-      <c r="S157" t="s">
+      <c r="T157" t="s">
         <v>918</v>
       </c>
     </row>
-    <row r="158" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E158" t="s">
+    <row r="158" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F158" t="s">
         <v>208</v>
       </c>
-      <c r="G158" t="s">
+      <c r="H158" t="s">
         <v>458</v>
       </c>
-      <c r="S158" t="s">
+      <c r="T158" t="s">
         <v>919</v>
       </c>
     </row>
-    <row r="159" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E159" t="s">
+    <row r="159" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F159" t="s">
         <v>209</v>
       </c>
-      <c r="G159" t="s">
+      <c r="H159" t="s">
         <v>459</v>
       </c>
-      <c r="S159" t="s">
+      <c r="T159" t="s">
         <v>920</v>
       </c>
     </row>
-    <row r="160" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E160" t="s">
+    <row r="160" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F160" t="s">
         <v>210</v>
       </c>
-      <c r="G160" t="s">
+      <c r="H160" t="s">
         <v>460</v>
       </c>
-      <c r="S160" t="s">
+      <c r="T160" t="s">
         <v>921</v>
       </c>
     </row>
-    <row r="161" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E161" t="s">
+    <row r="161" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F161" t="s">
         <v>211</v>
       </c>
-      <c r="G161" t="s">
+      <c r="H161" t="s">
         <v>461</v>
       </c>
-      <c r="S161" t="s">
+      <c r="T161" t="s">
         <v>922</v>
       </c>
     </row>
-    <row r="162" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E162" t="s">
+    <row r="162" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F162" t="s">
         <v>212</v>
       </c>
-      <c r="G162" t="s">
+      <c r="H162" t="s">
         <v>462</v>
       </c>
-      <c r="S162" t="s">
+      <c r="T162" t="s">
         <v>923</v>
       </c>
     </row>
-    <row r="163" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E163" t="s">
+    <row r="163" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F163" t="s">
         <v>213</v>
       </c>
-      <c r="G163" t="s">
+      <c r="H163" t="s">
         <v>463</v>
       </c>
-      <c r="S163" t="s">
+      <c r="T163" t="s">
         <v>924</v>
       </c>
     </row>
-    <row r="164" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E164" t="s">
+    <row r="164" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F164" t="s">
         <v>214</v>
       </c>
-      <c r="G164" t="s">
+      <c r="H164" t="s">
         <v>464</v>
       </c>
-      <c r="S164" t="s">
+      <c r="T164" t="s">
         <v>925</v>
       </c>
     </row>
-    <row r="165" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E165" t="s">
+    <row r="165" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F165" t="s">
         <v>215</v>
       </c>
-      <c r="G165" t="s">
+      <c r="H165" t="s">
         <v>465</v>
       </c>
-      <c r="S165" t="s">
+      <c r="T165" t="s">
         <v>926</v>
       </c>
     </row>
-    <row r="166" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E166" t="s">
+    <row r="166" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F166" t="s">
         <v>216</v>
       </c>
-      <c r="G166" t="s">
+      <c r="H166" t="s">
         <v>466</v>
       </c>
-      <c r="S166" t="s">
+      <c r="T166" t="s">
         <v>927</v>
       </c>
     </row>
-    <row r="167" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E167" t="s">
+    <row r="167" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F167" t="s">
         <v>217</v>
       </c>
-      <c r="G167" t="s">
+      <c r="H167" t="s">
         <v>467</v>
       </c>
-      <c r="S167" t="s">
+      <c r="T167" t="s">
         <v>928</v>
       </c>
     </row>
-    <row r="168" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E168" t="s">
+    <row r="168" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F168" t="s">
         <v>218</v>
       </c>
-      <c r="G168" t="s">
+      <c r="H168" t="s">
         <v>468</v>
       </c>
-      <c r="S168" t="s">
+      <c r="T168" t="s">
         <v>929</v>
       </c>
     </row>
-    <row r="169" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E169" t="s">
+    <row r="169" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F169" t="s">
         <v>219</v>
       </c>
-      <c r="S169" t="s">
+      <c r="T169" t="s">
         <v>930</v>
       </c>
     </row>
-    <row r="170" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E170" t="s">
+    <row r="170" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F170" t="s">
         <v>220</v>
       </c>
-      <c r="S170" t="s">
+      <c r="T170" t="s">
         <v>931</v>
       </c>
     </row>
-    <row r="171" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E171" t="s">
+    <row r="171" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F171" t="s">
         <v>221</v>
       </c>
-      <c r="S171" t="s">
+      <c r="T171" t="s">
         <v>932</v>
       </c>
     </row>
-    <row r="172" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E172" t="s">
+    <row r="172" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F172" t="s">
         <v>222</v>
       </c>
-      <c r="S172" t="s">
+      <c r="T172" t="s">
         <v>933</v>
       </c>
     </row>
-    <row r="173" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E173" t="s">
+    <row r="173" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F173" t="s">
         <v>223</v>
       </c>
-      <c r="S173" t="s">
+      <c r="T173" t="s">
         <v>934</v>
       </c>
     </row>
-    <row r="174" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E174" t="s">
+    <row r="174" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F174" t="s">
         <v>224</v>
       </c>
-      <c r="S174" t="s">
+      <c r="T174" t="s">
         <v>935</v>
       </c>
     </row>
-    <row r="175" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E175" t="s">
+    <row r="175" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F175" t="s">
         <v>225</v>
       </c>
-      <c r="S175" t="s">
+      <c r="T175" t="s">
         <v>936</v>
       </c>
     </row>
-    <row r="176" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E176" t="s">
+    <row r="176" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F176" t="s">
         <v>226</v>
       </c>
-      <c r="S176" t="s">
+      <c r="T176" t="s">
         <v>937</v>
       </c>
     </row>
-    <row r="177" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E177" t="s">
+    <row r="177" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F177" t="s">
         <v>227</v>
       </c>
-      <c r="S177" t="s">
+      <c r="T177" t="s">
         <v>938</v>
       </c>
     </row>
-    <row r="178" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E178" t="s">
+    <row r="178" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F178" t="s">
         <v>228</v>
       </c>
-      <c r="S178" t="s">
+      <c r="T178" t="s">
         <v>939</v>
       </c>
     </row>
-    <row r="179" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E179" t="s">
+    <row r="179" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F179" t="s">
         <v>229</v>
       </c>
-      <c r="S179" t="s">
+      <c r="T179" t="s">
         <v>940</v>
       </c>
     </row>
-    <row r="180" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E180" t="s">
+    <row r="180" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F180" t="s">
         <v>230</v>
       </c>
-      <c r="S180" t="s">
+      <c r="T180" t="s">
         <v>941</v>
       </c>
     </row>
-    <row r="181" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E181" t="s">
+    <row r="181" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F181" t="s">
         <v>231</v>
       </c>
-      <c r="S181" t="s">
+      <c r="T181" t="s">
         <v>942</v>
       </c>
     </row>
-    <row r="182" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E182" t="s">
+    <row r="182" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F182" t="s">
         <v>232</v>
       </c>
-      <c r="S182" t="s">
+      <c r="T182" t="s">
         <v>943</v>
       </c>
     </row>
-    <row r="183" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E183" t="s">
+    <row r="183" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F183" t="s">
         <v>233</v>
       </c>
-      <c r="S183" t="s">
+      <c r="T183" t="s">
         <v>944</v>
       </c>
     </row>
-    <row r="184" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E184" t="s">
+    <row r="184" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F184" t="s">
         <v>234</v>
       </c>
-      <c r="S184" t="s">
+      <c r="T184" t="s">
         <v>945</v>
       </c>
     </row>
-    <row r="185" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E185" t="s">
+    <row r="185" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F185" t="s">
         <v>235</v>
       </c>
-      <c r="S185" t="s">
+      <c r="T185" t="s">
         <v>946</v>
       </c>
     </row>
-    <row r="186" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E186" t="s">
+    <row r="186" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F186" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="187" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E187" t="s">
+    <row r="187" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F187" t="s">
         <v>237</v>
       </c>
     </row>
-    <row r="188" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E188" t="s">
+    <row r="188" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F188" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="189" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E189" t="s">
+    <row r="189" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F189" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="190" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E190" t="s">
+    <row r="190" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F190" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="191" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E191" t="s">
+    <row r="191" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F191" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="192" spans="5:19" x14ac:dyDescent="0.25">
-      <c r="E192" t="s">
+    <row r="192" spans="6:20" x14ac:dyDescent="0.25">
+      <c r="F192" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="193" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E193" t="s">
+    <row r="193" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F193" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="194" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E194" t="s">
+    <row r="194" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F194" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="195" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E195" t="s">
+    <row r="195" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F195" t="s">
         <v>245</v>
       </c>
     </row>
-    <row r="196" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E196" t="s">
+    <row r="196" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F196" t="s">
         <v>246</v>
       </c>
     </row>
-    <row r="197" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E197" t="s">
+    <row r="197" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F197" t="s">
         <v>247</v>
       </c>
     </row>
-    <row r="198" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E198" t="s">
+    <row r="198" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F198" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="199" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E199" t="s">
+    <row r="199" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F199" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="200" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E200" t="s">
+    <row r="200" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F200" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="201" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E201" t="s">
+    <row r="201" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F201" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="202" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E202" t="s">
+    <row r="202" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F202" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="203" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E203" t="s">
+    <row r="203" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F203" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="204" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E204" t="s">
+    <row r="204" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F204" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="205" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E205" t="s">
+    <row r="205" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F205" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="206" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E206" t="s">
+    <row r="206" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F206" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="207" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E207" t="s">
+    <row r="207" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F207" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="208" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E208" t="s">
+    <row r="208" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F208" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="209" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E209" t="s">
+    <row r="209" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F209" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="210" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E210" t="s">
+    <row r="210" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F210" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="211" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E211" t="s">
+    <row r="211" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F211" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="212" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E212" t="s">
+    <row r="212" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F212" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="213" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E213" t="s">
+    <row r="213" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F213" t="s">
         <v>263</v>
       </c>
     </row>
-    <row r="214" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E214" t="s">
+    <row r="214" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F214" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="215" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E215" t="s">
+    <row r="215" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F215" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="216" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E216" t="s">
+    <row r="216" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F216" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="217" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E217" t="s">
+    <row r="217" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F217" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="218" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E218" t="s">
+    <row r="218" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F218" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="219" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E219" t="s">
+    <row r="219" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F219" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="220" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E220" t="s">
+    <row r="220" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F220" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="221" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E221" t="s">
+    <row r="221" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F221" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="222" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E222" t="s">
+    <row r="222" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F222" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="223" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E223" t="s">
+    <row r="223" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F223" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="224" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E224" t="s">
+    <row r="224" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F224" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="225" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E225" t="s">
+    <row r="225" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F225" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="226" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E226" t="s">
+    <row r="226" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F226" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="227" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E227" t="s">
+    <row r="227" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F227" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="228" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E228" t="s">
+    <row r="228" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F228" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="229" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E229" t="s">
+    <row r="229" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F229" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="230" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E230" t="s">
+    <row r="230" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F230" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="231" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E231" t="s">
+    <row r="231" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F231" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="232" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E232" t="s">
+    <row r="232" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F232" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="233" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E233" t="s">
+    <row r="233" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F233" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="234" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E234" t="s">
+    <row r="234" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F234" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="235" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E235" t="s">
+    <row r="235" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F235" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="236" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E236" t="s">
+    <row r="236" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F236" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="237" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E237" t="s">
+    <row r="237" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F237" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="238" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E238" t="s">
+    <row r="238" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F238" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="239" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E239" t="s">
+    <row r="239" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F239" t="s">
         <v>289</v>
       </c>
     </row>
-    <row r="240" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E240" t="s">
+    <row r="240" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F240" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="241" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E241" t="s">
+    <row r="241" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F241" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="242" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E242" t="s">
+    <row r="242" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F242" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="243" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E243" t="s">
+    <row r="243" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F243" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="244" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E244" t="s">
+    <row r="244" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F244" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="245" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E245" t="s">
+    <row r="245" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F245" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="246" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E246" t="s">
+    <row r="246" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F246" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="247" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E247" t="s">
+    <row r="247" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F247" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="248" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E248" t="s">
+    <row r="248" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F248" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="249" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E249" t="s">
+    <row r="249" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F249" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="250" spans="5:5" x14ac:dyDescent="0.25">
-      <c r="E250" t="s">
+    <row r="250" spans="6:6" x14ac:dyDescent="0.25">
+      <c r="F250" t="s">
         <v>300</v>
       </c>
     </row>

</xml_diff>